<commit_message>
changes made only package matplotlib problem
</commit_message>
<xml_diff>
--- a/dataset/Maqsad_User_Profiles_Data.xlsx
+++ b/dataset/Maqsad_User_Profiles_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\techminds\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\techminds\Downloads\rameel-pro\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFBB98A7-5FC6-4C47-9D40-36829F2AE4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55BFBA4-8B20-444F-99CF-6770912B99D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,24 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="41">
   <si>
-    <t>User_ID</t>
-  </si>
-  <si>
-    <t>Age_Group</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Educational_Board</t>
-  </si>
-  <si>
-    <t>Primary_Subject</t>
-  </si>
-  <si>
     <t>Feature_Usage</t>
   </si>
   <si>
@@ -148,6 +130,24 @@
   </si>
   <si>
     <t>DoubtSolve, Notes</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>age_group</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>educational_board</t>
+  </si>
+  <si>
+    <t>primary_subject</t>
   </si>
 </sst>
 </file>
@@ -411,8 +411,8 @@
   </sheetPr>
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -427,31 +427,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -459,28 +459,28 @@
         <v>501</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1">
         <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -488,28 +488,28 @@
         <v>502</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1">
         <v>60</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -517,28 +517,28 @@
         <v>503</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1">
         <v>20</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -546,28 +546,28 @@
         <v>504</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1">
         <v>35</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -575,28 +575,28 @@
         <v>505</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H6" s="1">
         <v>50</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -604,28 +604,28 @@
         <v>506</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H7" s="1">
         <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -633,28 +633,28 @@
         <v>507</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H8" s="1">
         <v>75</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -662,28 +662,28 @@
         <v>508</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H9" s="1">
         <v>90</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -691,28 +691,28 @@
         <v>509</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1">
         <v>40</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -720,28 +720,28 @@
         <v>510</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H11" s="1">
         <v>65</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -749,28 +749,28 @@
         <v>511</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H12" s="1">
         <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -778,28 +778,28 @@
         <v>512</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H13" s="1">
         <v>50</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -807,28 +807,28 @@
         <v>513</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1">
         <v>30</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -836,28 +836,28 @@
         <v>514</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H15" s="1">
         <v>70</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -865,28 +865,28 @@
         <v>515</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H16" s="1">
         <v>85</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -894,28 +894,28 @@
         <v>516</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H17" s="1">
         <v>40</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -923,28 +923,28 @@
         <v>517</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H18" s="1">
         <v>55</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -952,28 +952,28 @@
         <v>518</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H19" s="1">
         <v>95</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -981,28 +981,28 @@
         <v>519</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="H20" s="1">
         <v>60</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1010,28 +1010,28 @@
         <v>520</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H21" s="1">
         <v>20</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1039,28 +1039,28 @@
         <v>521</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H22" s="1">
         <v>45</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1068,28 +1068,28 @@
         <v>522</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H23" s="1">
         <v>35</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1097,28 +1097,28 @@
         <v>523</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H24" s="1">
         <v>80</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1126,28 +1126,28 @@
         <v>524</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H25" s="1">
         <v>50</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1155,28 +1155,28 @@
         <v>525</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G26" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H26" s="1">
         <v>25</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1184,28 +1184,28 @@
         <v>526</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H27" s="1">
         <v>90</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1213,28 +1213,28 @@
         <v>527</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H28" s="1">
         <v>30</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1242,28 +1242,28 @@
         <v>528</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H29" s="1">
         <v>40</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1271,28 +1271,28 @@
         <v>529</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H30" s="1">
         <v>65</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1300,28 +1300,28 @@
         <v>530</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H31" s="1">
         <v>55</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1329,28 +1329,28 @@
         <v>531</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H32" s="1">
         <v>35</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1358,28 +1358,28 @@
         <v>532</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H33" s="1">
         <v>50</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1387,28 +1387,28 @@
         <v>533</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H34" s="1">
         <v>75</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1416,28 +1416,28 @@
         <v>534</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H35" s="1">
         <v>20</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1445,28 +1445,28 @@
         <v>535</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H36" s="1">
         <v>45</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -1474,28 +1474,28 @@
         <v>536</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H37" s="1">
         <v>60</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -1503,28 +1503,28 @@
         <v>537</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H38" s="1">
         <v>85</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -1532,28 +1532,28 @@
         <v>538</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H39" s="1">
         <v>30</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -1561,28 +1561,28 @@
         <v>539</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H40" s="1">
         <v>90</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1590,28 +1590,28 @@
         <v>540</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H41" s="1">
         <v>55</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1619,28 +1619,28 @@
         <v>541</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H42" s="1">
         <v>40</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -1648,28 +1648,28 @@
         <v>542</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G43" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H43" s="1">
         <v>25</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -1677,28 +1677,28 @@
         <v>543</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H44" s="1">
         <v>80</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -1706,28 +1706,28 @@
         <v>544</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H45" s="1">
         <v>35</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -1735,28 +1735,28 @@
         <v>545</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H46" s="1">
         <v>50</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -1764,28 +1764,28 @@
         <v>546</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H47" s="1">
         <v>95</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -1793,28 +1793,28 @@
         <v>547</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H48" s="1">
         <v>60</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -1822,28 +1822,28 @@
         <v>548</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H49" s="1">
         <v>20</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -1851,28 +1851,28 @@
         <v>549</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H50" s="1">
         <v>75</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -1880,28 +1880,28 @@
         <v>550</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H51" s="1">
         <v>45</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -1909,28 +1909,28 @@
         <v>551</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H52" s="1">
         <v>85</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -1938,28 +1938,28 @@
         <v>552</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G53" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H53" s="1">
         <v>40</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -1967,28 +1967,28 @@
         <v>553</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H54" s="1">
         <v>30</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -1996,28 +1996,28 @@
         <v>554</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H55" s="1">
         <v>90</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -2025,28 +2025,28 @@
         <v>555</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H56" s="1">
         <v>25</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -2054,28 +2054,28 @@
         <v>556</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H57" s="1">
         <v>55</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -2083,28 +2083,28 @@
         <v>557</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H58" s="1">
         <v>100</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -2112,28 +2112,28 @@
         <v>558</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H59" s="1">
         <v>65</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -2141,28 +2141,28 @@
         <v>559</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H60" s="1">
         <v>35</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -2170,28 +2170,28 @@
         <v>560</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H61" s="1">
         <v>95</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -2199,28 +2199,28 @@
         <v>561</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H62" s="1">
         <v>20</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -2228,28 +2228,28 @@
         <v>562</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G63" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H63" s="1">
         <v>45</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -2257,28 +2257,28 @@
         <v>563</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H64" s="1">
         <v>50</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -2286,28 +2286,28 @@
         <v>564</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H65" s="1">
         <v>70</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -2315,28 +2315,28 @@
         <v>565</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H66" s="1">
         <v>85</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -2344,28 +2344,28 @@
         <v>566</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H67" s="1">
         <v>30</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -2373,28 +2373,28 @@
         <v>567</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H68" s="1">
         <v>55</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -2402,28 +2402,28 @@
         <v>568</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F69" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H69" s="1">
         <v>90</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -2431,28 +2431,28 @@
         <v>569</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H70" s="1">
         <v>40</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -2460,28 +2460,28 @@
         <v>570</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H71" s="1">
         <v>65</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -2489,28 +2489,28 @@
         <v>571</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H72" s="1">
         <v>100</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -2518,28 +2518,28 @@
         <v>572</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H73" s="1">
         <v>75</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -2547,28 +2547,28 @@
         <v>573</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H74" s="1">
         <v>35</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -2576,28 +2576,28 @@
         <v>574</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H75" s="1">
         <v>25</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -2605,28 +2605,28 @@
         <v>575</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H76" s="1">
         <v>40</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -2634,28 +2634,28 @@
         <v>576</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H77" s="1">
         <v>95</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -2663,28 +2663,28 @@
         <v>577</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H78" s="1">
         <v>60</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -2692,28 +2692,28 @@
         <v>578</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H79" s="1">
         <v>20</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -2721,28 +2721,28 @@
         <v>579</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H80" s="1">
         <v>70</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -2750,28 +2750,28 @@
         <v>580</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H81" s="1">
         <v>50</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -2779,28 +2779,28 @@
         <v>581</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H82" s="1">
         <v>30</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -2808,28 +2808,28 @@
         <v>582</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H83" s="1">
         <v>55</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -2837,28 +2837,28 @@
         <v>583</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H84" s="1">
         <v>85</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -2866,28 +2866,28 @@
         <v>584</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H85" s="1">
         <v>40</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -2895,28 +2895,28 @@
         <v>585</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H86" s="1">
         <v>65</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -2924,28 +2924,28 @@
         <v>586</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H87" s="1">
         <v>75</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
@@ -2953,28 +2953,28 @@
         <v>587</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F88" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H88" s="1">
         <v>100</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
@@ -2982,28 +2982,28 @@
         <v>588</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H89" s="1">
         <v>25</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
@@ -3011,28 +3011,28 @@
         <v>589</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G90" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H90" s="1">
         <v>35</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3040,28 +3040,28 @@
         <v>590</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F91" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G91" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H91" s="1">
         <v>90</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3069,28 +3069,28 @@
         <v>591</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H92" s="1">
         <v>50</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
@@ -3098,28 +3098,28 @@
         <v>592</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H93" s="1">
         <v>40</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -3127,28 +3127,28 @@
         <v>593</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F94" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G94" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H94" s="1">
         <v>80</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
@@ -3156,28 +3156,28 @@
         <v>594</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H95" s="1">
         <v>30</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -3185,28 +3185,28 @@
         <v>595</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H96" s="1">
         <v>55</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -3214,28 +3214,28 @@
         <v>596</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F97" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G97" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H97" s="1">
         <v>95</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -3243,28 +3243,28 @@
         <v>597</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H98" s="1">
         <v>60</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
@@ -3272,28 +3272,28 @@
         <v>598</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H99" s="1">
         <v>25</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
@@ -3301,28 +3301,28 @@
         <v>599</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H100" s="1">
         <v>35</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -3330,28 +3330,28 @@
         <v>600</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H101" s="1">
         <v>90</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>